<commit_message>
Final version for base framework
</commit_message>
<xml_diff>
--- a/src/test/resources/customer_data/CustomerTransactions.xlsx
+++ b/src/test/resources/customer_data/CustomerTransactions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t>Item Code</t>
   </si>
@@ -119,18 +119,9 @@
     <t>Payment amount</t>
   </si>
   <si>
-    <t>I-VS004000163</t>
-  </si>
-  <si>
     <t>Full</t>
   </si>
   <si>
-    <t>I-VS004000165</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
     <t>Cash</t>
   </si>
   <si>
@@ -170,13 +161,28 @@
     <t>6567452</t>
   </si>
   <si>
-    <t>05 June 2018</t>
-  </si>
-  <si>
     <t>07 July 2018</t>
   </si>
   <si>
     <t xml:space="preserve">EMIRATES ISLAMIC </t>
+  </si>
+  <si>
+    <t>I-VS004002270</t>
+  </si>
+  <si>
+    <t>I-VS004002271</t>
+  </si>
+  <si>
+    <t>7842.88</t>
+  </si>
+  <si>
+    <t>12000</t>
+  </si>
+  <si>
+    <t>8000</t>
+  </si>
+  <si>
+    <t>27 June 2018</t>
   </si>
 </sst>
 </file>
@@ -226,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -248,6 +254,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,7 +688,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -804,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,19 +832,19 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
+      <c r="A2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>34</v>
+        <v>48</v>
+      </c>
+      <c r="B3" s="11">
+        <v>25000</v>
       </c>
     </row>
   </sheetData>
@@ -848,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,64 +879,64 @@
         <v>30</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2">
-        <v>77.58</v>
+        <v>32</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3">
-        <v>75</v>
+        <v>34</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>42</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="B4">
-        <v>25</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding : 1) Reading Configurations from sqlite 2) Reading Account Data (Credit Limit , Balance) with Tolerance 3) Implementing Credit Limit Check with Tolerance 4) Changes on TestNG Suit Xml file to handle multple test for the same metod
</commit_message>
<xml_diff>
--- a/src/test/resources/customer_data/CustomerTransactions.xlsx
+++ b/src/test/resources/customer_data/CustomerTransactions.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="4" r:id="rId1"/>
-    <sheet name="Returns" sheetId="5" r:id="rId2"/>
-    <sheet name="PG1" sheetId="6" r:id="rId3"/>
-    <sheet name="PG2" sheetId="7" r:id="rId4"/>
+    <sheet name="PG1" sheetId="6" r:id="rId2"/>
+    <sheet name="PG2" sheetId="7" r:id="rId3"/>
+    <sheet name="Returns" sheetId="5" r:id="rId4"/>
     <sheet name="Invoices to collect" sheetId="8" r:id="rId5"/>
     <sheet name="Payment methods" sheetId="10" r:id="rId6"/>
   </sheets>
@@ -179,13 +179,13 @@
     <t>7842.08</t>
   </si>
   <si>
-    <t>07 August 2018</t>
-  </si>
-  <si>
     <t>23 July 2018</t>
   </si>
   <si>
     <t>I-VS004002291</t>
+  </si>
+  <si>
+    <t>27 August 2018</t>
   </si>
 </sst>
 </file>
@@ -540,7 +540,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,107 +616,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>4001</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>4002</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>4002</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -768,7 +667,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -809,11 +708,112 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>4001</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>4002</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>4002</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -849,7 +849,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="2">
         <v>26675</v>
@@ -865,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +924,7 @@
         <v>39</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -944,7 +944,7 @@
         <v>44</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding : 1) Update Appium to Latest Version 2) Adding Delivery Screen with complementary Order 3) Adding Sorting List and Order List methods 4) Adding Tesseract Client to Convert Images to text 5) Adding Delete Item common feature (Currently Only used in Delivery) 6) Adding Taking Screenshot method 7) Adding Route General Data to get these data and always have it ready to be used 8) Adding Predicting Document Sequence for next transaction 9) Adding check saved SQLite data for orders (Currently Only used in complementary order)
</commit_message>
<xml_diff>
--- a/src/test/resources/customer_data/CustomerTransactions.xlsx
+++ b/src/test/resources/customer_data/CustomerTransactions.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="4" r:id="rId1"/>
     <sheet name="PG1" sheetId="6" r:id="rId2"/>
     <sheet name="PG2" sheetId="7" r:id="rId3"/>
     <sheet name="Returns" sheetId="5" r:id="rId4"/>
-    <sheet name="Invoices to collect" sheetId="8" r:id="rId5"/>
-    <sheet name="Payment methods" sheetId="10" r:id="rId6"/>
+    <sheet name="Delivery" sheetId="12" r:id="rId5"/>
+    <sheet name="Invoices to collect" sheetId="8" r:id="rId6"/>
+    <sheet name="Payment methods" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="76">
   <si>
     <t>Item Code</t>
   </si>
@@ -125,9 +126,6 @@
     <t>Cash</t>
   </si>
   <si>
-    <t>30 August 2018</t>
-  </si>
-  <si>
     <t>CDC</t>
   </si>
   <si>
@@ -164,9 +162,6 @@
     <t xml:space="preserve">EMIRATES ISLAMIC </t>
   </si>
   <si>
-    <t>12000</t>
-  </si>
-  <si>
     <t>8000</t>
   </si>
   <si>
@@ -179,20 +174,92 @@
     <t>7842.08</t>
   </si>
   <si>
-    <t>23 July 2018</t>
-  </si>
-  <si>
-    <t>I-VS004002291</t>
-  </si>
-  <si>
-    <t>27 August 2018</t>
+    <t>Promoted Discount (Value-Type)</t>
+  </si>
+  <si>
+    <t>23 August 2018</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>Order Quantity</t>
+  </si>
+  <si>
+    <t>4023</t>
+  </si>
+  <si>
+    <t>New Quantity</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Promoted Discount</t>
+  </si>
+  <si>
+    <t>Promotion</t>
+  </si>
+  <si>
+    <t>10-%</t>
+  </si>
+  <si>
+    <t>1.5-ABC</t>
+  </si>
+  <si>
+    <t>Discount-Type</t>
+  </si>
+  <si>
+    <t>5-%</t>
+  </si>
+  <si>
+    <t>Original Net Total</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t>New Promotions</t>
+  </si>
+  <si>
+    <t>New Promoted Discount</t>
+  </si>
+  <si>
+    <t>Pack</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>30 November 2018</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>I-VS004002297</t>
+  </si>
+  <si>
+    <t>15 November 2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +280,12 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -235,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -257,6 +330,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,18 +622,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -558,8 +644,20 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
@@ -569,8 +667,20 @@
       <c r="C2" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>17</v>
       </c>
@@ -580,8 +690,20 @@
       <c r="C3" s="7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>17</v>
       </c>
@@ -591,8 +713,20 @@
       <c r="C4" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
@@ -602,7 +736,7 @@
       <c r="C5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -713,7 +847,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,7 +915,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -811,10 +945,316 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="2">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="2">
+        <v>120</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="2">
+        <v>5</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="2">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="2">
+        <v>5</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="11">
+        <v>15</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="2">
+        <v>144</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="2">
+        <v>5</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4023</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="14">
+        <v>0</v>
+      </c>
+      <c r="D6" s="14">
+        <v>17</v>
+      </c>
+      <c r="E6" s="14">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="2">
+        <v>5</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>4023</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="14">
+        <v>0</v>
+      </c>
+      <c r="D7" s="14">
+        <v>39</v>
+      </c>
+      <c r="E7" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2">
+        <v>9</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="11">
+        <v>15</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="2">
+        <v>35931.94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,7 +1273,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>31</v>
@@ -841,7 +1281,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>31</v>
@@ -849,10 +1289,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B4" s="2">
-        <v>26675</v>
+        <v>24675</v>
       </c>
     </row>
   </sheetData>
@@ -861,12 +1301,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,16 +1327,16 @@
         <v>30</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="E1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -904,47 +1344,47 @@
         <v>32</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
       <c r="E3" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>44</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>